<commit_message>
accidental save, but no changes were made to files
</commit_message>
<xml_diff>
--- a/data/RespirationRate/Block1_Day29_plate2_results_Oxygen.xlsx
+++ b/data/RespirationRate/Block1_Day29_plate2_results_Oxygen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreSens\SDR_v4.0.0\Resource Quality Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/mlfearon_umich_edu/Documents/PROJECTS/MHMP Daphnia Duffy/Resource Quality/Data and Code/resource-quality-expt/data/RespirationRate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB521328-6ABB-4E35-A08F-30E422365DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{BB521328-6ABB-4E35-A08F-30E422365DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFE444A2-D48E-465E-B5B7-1468CD4EE05B}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="16875" windowHeight="10523" xr2:uid="{56002A76-AEA1-4BC8-A660-D9CCD83646C9}"/>
+    <workbookView xWindow="30030" yWindow="3195" windowWidth="21600" windowHeight="11265" xr2:uid="{56002A76-AEA1-4BC8-A660-D9CCD83646C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Oxygen Orginal" sheetId="2" r:id="rId1"/>
@@ -827,11 +827,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2560-1510-42BE-9063-629A3CFF0F77}">
   <dimension ref="A1:AF88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A1:XFD12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -860,7 +862,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -874,7 +876,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -888,7 +890,7 @@
         <v>54.4</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -908,7 +910,7 @@
         <v>46.95</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -922,7 +924,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -936,7 +938,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
         <v>27</v>
       </c>
@@ -944,7 +946,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
         <v>28</v>
       </c>
@@ -952,7 +954,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1047,7 +1049,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1139,7 +1141,7 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1231,7 +1233,7 @@
         <v>21.97</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1323,7 +1325,7 @@
         <v>22.02</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1415,7 +1417,7 @@
         <v>22.06</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -1507,7 +1509,7 @@
         <v>22.09</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -1599,7 +1601,7 @@
         <v>22.11</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1691,7 +1693,7 @@
         <v>22.13</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -1783,7 +1785,7 @@
         <v>22.13</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1875,7 +1877,7 @@
         <v>22.16</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -1967,7 +1969,7 @@
         <v>22.15</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -2059,7 +2061,7 @@
         <v>22.15</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -2151,7 +2153,7 @@
         <v>22.15</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -2243,7 +2245,7 @@
         <v>22.13</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -2335,7 +2337,7 @@
         <v>22.11</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -2427,7 +2429,7 @@
         <v>22.11</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -2519,7 +2521,7 @@
         <v>22.09</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -2611,7 +2613,7 @@
         <v>22.09</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -2703,7 +2705,7 @@
         <v>22.08</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -2795,7 +2797,7 @@
         <v>22.06</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2887,7 +2889,7 @@
         <v>22.06</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>81</v>
       </c>
@@ -2979,7 +2981,7 @@
         <v>22.04</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -3071,7 +3073,7 @@
         <v>22.02</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -3163,7 +3165,7 @@
         <v>22.02</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>84</v>
       </c>
@@ -3255,7 +3257,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -3347,7 +3349,7 @@
         <v>21.99</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -3439,7 +3441,7 @@
         <v>21.99</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -3531,7 +3533,7 @@
         <v>21.98</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -3623,7 +3625,7 @@
         <v>21.97</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>89</v>
       </c>
@@ -3715,7 +3717,7 @@
         <v>21.95</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>90</v>
       </c>
@@ -3807,7 +3809,7 @@
         <v>21.95</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -3899,7 +3901,7 @@
         <v>21.93</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -3991,7 +3993,7 @@
         <v>21.93</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -4083,7 +4085,7 @@
         <v>21.93</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -4175,7 +4177,7 @@
         <v>21.91</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -4267,7 +4269,7 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -4359,7 +4361,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>97</v>
       </c>
@@ -4451,7 +4453,7 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -4543,7 +4545,7 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>99</v>
       </c>
@@ -4635,7 +4637,7 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -4727,7 +4729,7 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>101</v>
       </c>
@@ -4819,7 +4821,7 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>102</v>
       </c>
@@ -4911,7 +4913,7 @@
         <v>21.84</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>103</v>
       </c>
@@ -5003,7 +5005,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>104</v>
       </c>
@@ -5095,7 +5097,7 @@
         <v>21.83</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>105</v>
       </c>
@@ -5187,7 +5189,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>106</v>
       </c>
@@ -5279,7 +5281,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>107</v>
       </c>
@@ -5371,7 +5373,7 @@
         <v>21.81</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>108</v>
       </c>
@@ -5463,7 +5465,7 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>109</v>
       </c>
@@ -5555,7 +5557,7 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>110</v>
       </c>
@@ -5647,7 +5649,7 @@
         <v>21.79</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>111</v>
       </c>
@@ -5739,7 +5741,7 @@
         <v>21.77</v>
       </c>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>112</v>
       </c>
@@ -5831,7 +5833,7 @@
         <v>21.77</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>113</v>
       </c>
@@ -5923,7 +5925,7 @@
         <v>21.77</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>114</v>
       </c>
@@ -6015,7 +6017,7 @@
         <v>21.77</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>115</v>
       </c>
@@ -6107,7 +6109,7 @@
         <v>21.77</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>116</v>
       </c>
@@ -6199,7 +6201,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>117</v>
       </c>
@@ -6291,7 +6293,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>118</v>
       </c>
@@ -6383,7 +6385,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>119</v>
       </c>
@@ -6475,7 +6477,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>120</v>
       </c>
@@ -6567,7 +6569,7 @@
         <v>21.74</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>121</v>
       </c>
@@ -6659,7 +6661,7 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>122</v>
       </c>
@@ -6751,7 +6753,7 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>123</v>
       </c>
@@ -6843,7 +6845,7 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>124</v>
       </c>
@@ -6935,7 +6937,7 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>125</v>
       </c>
@@ -7027,7 +7029,7 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>126</v>
       </c>
@@ -7119,7 +7121,7 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>127</v>
       </c>
@@ -7211,7 +7213,7 @@
         <v>21.73</v>
       </c>
     </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>128</v>
       </c>
@@ -7303,7 +7305,7 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>129</v>
       </c>
@@ -7395,7 +7397,7 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>130</v>
       </c>
@@ -7487,7 +7489,7 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>131</v>
       </c>
@@ -7579,7 +7581,7 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>132</v>
       </c>
@@ -7671,7 +7673,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>133</v>
       </c>
@@ -7763,7 +7765,7 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>134</v>
       </c>
@@ -7855,7 +7857,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>135</v>
       </c>
@@ -7958,7 +7960,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>